<commit_message>
Compatibility for missing data in output excel
</commit_message>
<xml_diff>
--- a/input_fake.xlsx
+++ b/input_fake.xlsx
@@ -52,7 +52,7 @@
     <t xml:space="preserve">impact</t>
   </si>
   <si>
-    <t xml:space="preserve">flex. Strenght</t>
+    <t xml:space="preserve">flex. Strength</t>
   </si>
   <si>
     <t xml:space="preserve">E-modulus</t>
@@ -266,10 +266,10 @@
   <dimension ref="A1:AMJ27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G11" activeCellId="0" sqref="G11"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.36"/>

</xml_diff>